<commit_message>
some fuel techs to PRE; spcool scaling for LT/LV/LU/EE; reporting options
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_zscaling.xlsx
+++ b/SuppXLS/Scen_zscaling.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\EU-TIMES\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B2BD9A-CF58-4B51-9E9A-0DD83B5159D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA32FCAA-E88F-47BE-9817-FE07CAAB0E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scaling" sheetId="27" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="28" r:id="rId2"/>
+    <sheet name="Retirement control" sheetId="28" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>Attribute</t>
   </si>
@@ -94,6 +94,51 @@
   </si>
   <si>
     <t>R_ES-FL-SpCool</t>
+  </si>
+  <si>
+    <t>*This is to control whether retirement and planned plants are used or not</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Attrib_Cond</t>
+  </si>
+  <si>
+    <t>Pset_PD</t>
+  </si>
+  <si>
+    <t>RCAP_BND</t>
+  </si>
+  <si>
+    <t>CAP_BND</t>
+  </si>
+  <si>
+    <t>Existing Elec*,Existing CHP*</t>
+  </si>
+  <si>
+    <t>ELCSOL,ELCWIN</t>
+  </si>
+  <si>
+    <t>-ELCSOL,-ELCWIN</t>
+  </si>
+  <si>
+    <t>-CAP_BND</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>* moved here so that it sees all scenarios for CAP_BND</t>
+  </si>
+  <si>
+    <t>LO</t>
   </si>
 </sst>
 </file>
@@ -2627,7 +2672,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="1789" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2644,6 +2689,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1790">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4773,7 +4819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE72BF17-55AF-466D-B3F7-A0457CBC06F4}">
   <dimension ref="A3:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -5251,12 +5297,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36AE299-60AD-4717-8B1F-1A2F97BEDEE7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2010</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2030</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2020</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>